<commit_message>
:construction: [functionalities] stabilization when bulk upload with db session and fix bugs when get fields from param
</commit_message>
<xml_diff>
--- a/test/test_employees1.xlsx
+++ b/test/test_employees1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ARCHIVOS\ARCHIVOS JOB\lib_gr_sqlmodel_xlsx\test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ARCHIVOS\ARCHIVOS JOB\my_libs\alchemymodel_xlsx\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,13 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
-  <si>
-    <t>gr_sql_model3@example.com</t>
-  </si>
-  <si>
-    <t>gr_sql_model4@example.com</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Email</t>
   </si>
@@ -45,7 +39,10 @@
     <t>No</t>
   </si>
   <si>
-    <t>gr_sql_model5@example.com</t>
+    <t>gr_sql_model1@example.com</t>
+  </si>
+  <si>
+    <t>gr_sql_model2@example.com</t>
   </si>
 </sst>
 </file>
@@ -430,10 +427,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -446,21 +443,21 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B2" s="4">
         <v>45017</v>
@@ -469,12 +466,12 @@
         <v>1500</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B3" s="4">
         <v>45018</v>
@@ -483,30 +480,15 @@
         <v>1500</v>
       </c>
       <c r="D3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="4">
-        <v>45019</v>
-      </c>
-      <c r="C4" s="5">
-        <v>1001</v>
-      </c>
-      <c r="D4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1"/>
     <hyperlink ref="A3" r:id="rId2"/>
-    <hyperlink ref="A4" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>